<commit_message>
added july 20 data
</commit_message>
<xml_diff>
--- a/Curr/TeamStats4_Curr.xlsx
+++ b/Curr/TeamStats4_Curr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/My codes/NBA/2019-2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/My codes/NBA_pred/Curr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BB557D-6DE5-6845-9669-62295746D2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF185554-7F30-B14D-BB24-F8A8F11C16E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16280" xr2:uid="{8431C8E5-BF9C-1542-B7C5-FA8A9E3CC57D}"/>
   </bookViews>
@@ -147,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +158,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
@@ -182,11 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B8DDE3-F9C0-F140-AF64-C426B74EEF4D}">
-  <dimension ref="A1:AE28"/>
+  <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A2:A6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,14 +618,14 @@
       <c r="B2" s="1">
         <v>0.26300000000000001</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.26800000000000002</v>
+      <c r="C2" s="4">
+        <v>0.45100000000000001</v>
       </c>
       <c r="D2" s="1">
         <v>0.25600000000000001</v>
       </c>
-      <c r="E2" s="1">
-        <v>0.29299999999999998</v>
+      <c r="E2" s="4">
+        <v>0.378</v>
       </c>
       <c r="F2" s="1">
         <v>0.255</v>
@@ -626,8 +633,8 @@
       <c r="G2" s="1">
         <v>0.23</v>
       </c>
-      <c r="H2" s="1">
-        <v>0.26900000000000002</v>
+      <c r="H2" s="4">
+        <v>0.33300000000000002</v>
       </c>
       <c r="I2" s="1">
         <v>0.29799999999999999</v>
@@ -659,8 +666,8 @@
       <c r="R2" s="1">
         <v>0.23899999999999999</v>
       </c>
-      <c r="S2" s="1">
-        <v>0.252</v>
+      <c r="S2" s="4">
+        <v>0.191</v>
       </c>
       <c r="T2" s="1">
         <v>0.23200000000000001</v>
@@ -706,14 +713,14 @@
       <c r="B3" s="1">
         <v>48.6</v>
       </c>
-      <c r="C3" s="1">
-        <v>50.9</v>
+      <c r="C3" s="4">
+        <v>54.1</v>
       </c>
       <c r="D3" s="1">
         <v>50.2</v>
       </c>
-      <c r="E3" s="1">
-        <v>50.3</v>
+      <c r="E3" s="4">
+        <v>45.7</v>
       </c>
       <c r="F3" s="1">
         <v>51</v>
@@ -721,8 +728,8 @@
       <c r="G3" s="1">
         <v>52.6</v>
       </c>
-      <c r="H3" s="1">
-        <v>51.4</v>
+      <c r="H3" s="4">
+        <v>48.4</v>
       </c>
       <c r="I3" s="1">
         <v>52.2</v>
@@ -754,8 +761,8 @@
       <c r="R3" s="1">
         <v>52.3</v>
       </c>
-      <c r="S3" s="1">
-        <v>53.1</v>
+      <c r="S3" s="4">
+        <v>48.8</v>
       </c>
       <c r="T3" s="1">
         <v>54</v>
@@ -801,14 +808,14 @@
       <c r="B4" s="1">
         <v>0.22</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.26</v>
+      <c r="C4" s="4">
+        <v>0.378</v>
       </c>
       <c r="D4" s="1">
         <v>0.26</v>
       </c>
-      <c r="E4" s="1">
-        <v>0.27500000000000002</v>
+      <c r="E4" s="4">
+        <v>0.45100000000000001</v>
       </c>
       <c r="F4" s="1">
         <v>0.27800000000000002</v>
@@ -816,8 +823,8 @@
       <c r="G4" s="1">
         <v>0.25600000000000001</v>
       </c>
-      <c r="H4" s="1">
-        <v>0.23400000000000001</v>
+      <c r="H4" s="4">
+        <v>0.191</v>
       </c>
       <c r="I4" s="1">
         <v>0.26700000000000002</v>
@@ -849,8 +856,8 @@
       <c r="R4" s="1">
         <v>0.26400000000000001</v>
       </c>
-      <c r="S4" s="1">
-        <v>0.26500000000000001</v>
+      <c r="S4" s="4">
+        <v>0.33300000000000002</v>
       </c>
       <c r="T4" s="1">
         <v>0.27900000000000003</v>
@@ -896,14 +903,14 @@
       <c r="B5" s="1">
         <v>13.5</v>
       </c>
-      <c r="C5" s="1">
-        <v>15.4</v>
+      <c r="C5" s="4">
+        <v>21.6</v>
       </c>
       <c r="D5" s="1">
         <v>16.600000000000001</v>
       </c>
-      <c r="E5" s="1">
-        <v>13.8</v>
+      <c r="E5" s="4">
+        <v>15.5</v>
       </c>
       <c r="F5" s="1">
         <v>15.2</v>
@@ -911,8 +918,8 @@
       <c r="G5" s="1">
         <v>14.5</v>
       </c>
-      <c r="H5" s="1">
-        <v>12.1</v>
+      <c r="H5" s="4">
+        <v>20.8</v>
       </c>
       <c r="I5" s="1">
         <v>13.7</v>
@@ -944,8 +951,8 @@
       <c r="R5" s="1">
         <v>12.5</v>
       </c>
-      <c r="S5" s="1">
-        <v>13.8</v>
+      <c r="S5" s="4">
+        <v>19.600000000000001</v>
       </c>
       <c r="T5" s="1">
         <v>15.1</v>
@@ -991,14 +998,14 @@
       <c r="B6" s="1">
         <v>22.4</v>
       </c>
-      <c r="C6" s="1">
-        <v>26.6</v>
+      <c r="C6" s="4">
+        <v>18.600000000000001</v>
       </c>
       <c r="D6" s="1">
         <v>28.5</v>
       </c>
-      <c r="E6" s="1">
-        <v>26.6</v>
+      <c r="E6" s="4">
+        <v>25.5</v>
       </c>
       <c r="F6" s="1">
         <v>26.8</v>
@@ -1006,8 +1013,8 @@
       <c r="G6" s="1">
         <v>27.3</v>
       </c>
-      <c r="H6" s="1">
-        <v>25.3</v>
+      <c r="H6" s="4">
+        <v>36.799999999999997</v>
       </c>
       <c r="I6" s="1">
         <v>24.4</v>
@@ -1039,8 +1046,8 @@
       <c r="R6" s="1">
         <v>29</v>
       </c>
-      <c r="S6" s="1">
-        <v>26.9</v>
+      <c r="S6" s="4">
+        <v>34</v>
       </c>
       <c r="T6" s="1">
         <v>26.5</v>
@@ -1079,247 +1086,93 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>